<commit_message>
Completed 2002, 2004, and 2014
</commit_message>
<xml_diff>
--- a/results/2012_reps_by_priority.xlsx
+++ b/results/2012_reps_by_priority.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F14F57E-12EF-4E45-A291-5E18510FD889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC0AC4-FEC3-194F-BB94-5605C1C8A74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27260" windowHeight="16940" xr2:uid="{F43BD5BF-1917-8F4C-A94A-1C3F14CB937D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_2012_reps_by_priority" localSheetId="0">Sheet1!$A$1:$F$167</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{BCAF91A6-C0E4-4A48-A16D-6FECCDE14951}" name="2012_reps_by_priority" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/alecramsay/Documents/dev/MM2/results/2012_reps_by_priority.csv" comma="1">
+    <textPr sourceFile="/Users/alecramsay/Documents/dev/MM2/results/2012_reps_by_priority.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -281,13 +281,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -614,7 +612,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K170" sqref="K170"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,19 +662,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>435</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="H2" s="6">
+      <c r="C2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="H2" s="4">
         <v>0.50849999999999995</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>201</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2">
         <f>ROUND(A2*H$2,0) -I2</f>
         <v>20</v>
       </c>
@@ -707,7 +705,7 @@
         <f>IF(E3="DEM",I2+1, I2)</f>
         <v>202</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <f t="shared" ref="J3:J66" si="0">ROUND(A3*H$2,0) -I3</f>
         <v>20</v>
       </c>
@@ -739,7 +737,7 @@
         <f t="shared" ref="I4:I67" si="1">IF(E4="DEM",I3+1, I3)</f>
         <v>203</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -771,7 +769,7 @@
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -803,7 +801,7 @@
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -835,7 +833,7 @@
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -867,7 +865,7 @@
         <f t="shared" si="1"/>
         <v>206</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -899,7 +897,7 @@
         <f t="shared" si="1"/>
         <v>206</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -931,7 +929,7 @@
         <f t="shared" si="1"/>
         <v>207</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -963,7 +961,7 @@
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -995,7 +993,7 @@
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1027,7 +1025,7 @@
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1059,7 +1057,7 @@
         <f t="shared" si="1"/>
         <v>209</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1091,7 +1089,7 @@
         <f t="shared" si="1"/>
         <v>209</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1123,7 +1121,7 @@
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1155,7 +1153,7 @@
         <f t="shared" si="1"/>
         <v>211</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1187,7 +1185,7 @@
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1219,7 +1217,7 @@
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1251,7 +1249,7 @@
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1283,7 +1281,7 @@
         <f t="shared" si="1"/>
         <v>214</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1315,7 +1313,7 @@
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1347,7 +1345,7 @@
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1379,7 +1377,7 @@
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1411,7 +1409,7 @@
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1443,7 +1441,7 @@
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1475,7 +1473,7 @@
         <f t="shared" si="1"/>
         <v>217</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1507,7 +1505,7 @@
         <f t="shared" si="1"/>
         <v>217</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1539,7 +1537,7 @@
         <f t="shared" si="1"/>
         <v>218</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1571,7 +1569,7 @@
         <f t="shared" si="1"/>
         <v>219</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1603,7 +1601,7 @@
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1635,7 +1633,7 @@
         <f t="shared" si="1"/>
         <v>221</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1667,7 +1665,7 @@
         <f t="shared" si="1"/>
         <v>222</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1699,7 +1697,7 @@
         <f t="shared" si="1"/>
         <v>223</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1731,7 +1729,7 @@
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1763,7 +1761,7 @@
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1795,7 +1793,7 @@
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1827,7 +1825,7 @@
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1859,7 +1857,7 @@
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1891,7 +1889,7 @@
         <f t="shared" si="1"/>
         <v>226</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1923,7 +1921,7 @@
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1955,7 +1953,7 @@
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1987,7 +1985,7 @@
         <f t="shared" si="1"/>
         <v>228</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2019,7 +2017,7 @@
         <f t="shared" si="1"/>
         <v>229</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2051,7 +2049,7 @@
         <f t="shared" si="1"/>
         <v>229</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2083,7 +2081,7 @@
         <f t="shared" si="1"/>
         <v>229</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2115,7 +2113,7 @@
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2147,7 +2145,7 @@
         <f t="shared" si="1"/>
         <v>231</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2179,7 +2177,7 @@
         <f t="shared" si="1"/>
         <v>232</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2211,7 +2209,7 @@
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2243,7 +2241,7 @@
         <f t="shared" si="1"/>
         <v>234</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2275,7 +2273,7 @@
         <f t="shared" si="1"/>
         <v>235</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2307,7 +2305,7 @@
         <f t="shared" si="1"/>
         <v>236</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2339,7 +2337,7 @@
         <f t="shared" si="1"/>
         <v>236</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2371,7 +2369,7 @@
         <f t="shared" si="1"/>
         <v>236</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2403,7 +2401,7 @@
         <f t="shared" si="1"/>
         <v>236</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2435,7 +2433,7 @@
         <f t="shared" si="1"/>
         <v>237</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2467,7 +2465,7 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-      <c r="J58" s="4">
+      <c r="J58">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2499,7 +2497,7 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-      <c r="J59" s="4">
+      <c r="J59">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2531,7 +2529,7 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-      <c r="J60" s="4">
+      <c r="J60">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2563,7 +2561,7 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-      <c r="J61" s="4">
+      <c r="J61">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2595,7 +2593,7 @@
         <f t="shared" si="1"/>
         <v>239</v>
       </c>
-      <c r="J62" s="4">
+      <c r="J62">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2627,7 +2625,7 @@
         <f t="shared" si="1"/>
         <v>239</v>
       </c>
-      <c r="J63" s="4">
+      <c r="J63">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2659,7 +2657,7 @@
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="J64" s="4">
+      <c r="J64">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2691,7 +2689,7 @@
         <f t="shared" si="1"/>
         <v>241</v>
       </c>
-      <c r="J65" s="4">
+      <c r="J65">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2723,7 +2721,7 @@
         <f t="shared" si="1"/>
         <v>242</v>
       </c>
-      <c r="J66" s="4">
+      <c r="J66">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2755,7 +2753,7 @@
         <f t="shared" si="1"/>
         <v>243</v>
       </c>
-      <c r="J67" s="4">
+      <c r="J67">
         <f t="shared" ref="J67:J130" si="3">ROUND(A67*H$2,0) -I67</f>
         <v>11</v>
       </c>
@@ -2787,7 +2785,7 @@
         <f t="shared" ref="I68:I131" si="4">IF(E68="DEM",I67+1, I67)</f>
         <v>244</v>
       </c>
-      <c r="J68" s="4">
+      <c r="J68">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -2819,7 +2817,7 @@
         <f t="shared" si="4"/>
         <v>245</v>
       </c>
-      <c r="J69" s="4">
+      <c r="J69">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2851,7 +2849,7 @@
         <f t="shared" si="4"/>
         <v>246</v>
       </c>
-      <c r="J70" s="4">
+      <c r="J70">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2883,7 +2881,7 @@
         <f t="shared" si="4"/>
         <v>246</v>
       </c>
-      <c r="J71" s="4">
+      <c r="J71">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2915,7 +2913,7 @@
         <f t="shared" si="4"/>
         <v>247</v>
       </c>
-      <c r="J72" s="4">
+      <c r="J72">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2947,7 +2945,7 @@
         <f t="shared" si="4"/>
         <v>247</v>
       </c>
-      <c r="J73" s="4">
+      <c r="J73">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2979,7 +2977,7 @@
         <f t="shared" si="4"/>
         <v>247</v>
       </c>
-      <c r="J74" s="4">
+      <c r="J74">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3011,7 +3009,7 @@
         <f t="shared" si="4"/>
         <v>248</v>
       </c>
-      <c r="J75" s="4">
+      <c r="J75">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3043,7 +3041,7 @@
         <f t="shared" si="4"/>
         <v>249</v>
       </c>
-      <c r="J76" s="4">
+      <c r="J76">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3075,7 +3073,7 @@
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="J77" s="4">
+      <c r="J77">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3107,7 +3105,7 @@
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="J78" s="4">
+      <c r="J78">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3139,7 +3137,7 @@
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="J79" s="4">
+      <c r="J79">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3171,7 +3169,7 @@
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="J80" s="4">
+      <c r="J80">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3203,7 +3201,7 @@
         <f t="shared" si="4"/>
         <v>251</v>
       </c>
-      <c r="J81" s="4">
+      <c r="J81">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3235,7 +3233,7 @@
         <f t="shared" si="4"/>
         <v>252</v>
       </c>
-      <c r="J82" s="4">
+      <c r="J82">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3267,7 +3265,7 @@
         <f t="shared" si="4"/>
         <v>253</v>
       </c>
-      <c r="J83" s="4">
+      <c r="J83">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3299,7 +3297,7 @@
         <f t="shared" si="4"/>
         <v>253</v>
       </c>
-      <c r="J84" s="4">
+      <c r="J84">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3331,7 +3329,7 @@
         <f t="shared" si="4"/>
         <v>253</v>
       </c>
-      <c r="J85" s="4">
+      <c r="J85">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3363,7 +3361,7 @@
         <f t="shared" si="4"/>
         <v>253</v>
       </c>
-      <c r="J86" s="4">
+      <c r="J86">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3395,7 +3393,7 @@
         <f t="shared" si="4"/>
         <v>253</v>
       </c>
-      <c r="J87" s="4">
+      <c r="J87">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3427,7 +3425,7 @@
         <f t="shared" si="4"/>
         <v>254</v>
       </c>
-      <c r="J88" s="4">
+      <c r="J88">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3459,7 +3457,7 @@
         <f t="shared" si="4"/>
         <v>254</v>
       </c>
-      <c r="J89" s="4">
+      <c r="J89">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3491,7 +3489,7 @@
         <f t="shared" si="4"/>
         <v>254</v>
       </c>
-      <c r="J90" s="4">
+      <c r="J90">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3523,7 +3521,7 @@
         <f t="shared" si="4"/>
         <v>254</v>
       </c>
-      <c r="J91" s="4">
+      <c r="J91">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3555,7 +3553,7 @@
         <f t="shared" si="4"/>
         <v>255</v>
       </c>
-      <c r="J92" s="4">
+      <c r="J92">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3587,7 +3585,7 @@
         <f t="shared" si="4"/>
         <v>256</v>
       </c>
-      <c r="J93" s="4">
+      <c r="J93">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3619,7 +3617,7 @@
         <f t="shared" si="4"/>
         <v>257</v>
       </c>
-      <c r="J94" s="4">
+      <c r="J94">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3651,7 +3649,7 @@
         <f t="shared" si="4"/>
         <v>257</v>
       </c>
-      <c r="J95" s="4">
+      <c r="J95">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3683,7 +3681,7 @@
         <f t="shared" si="4"/>
         <v>257</v>
       </c>
-      <c r="J96" s="4">
+      <c r="J96">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3715,7 +3713,7 @@
         <f t="shared" si="4"/>
         <v>258</v>
       </c>
-      <c r="J97" s="4">
+      <c r="J97">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3747,7 +3745,7 @@
         <f t="shared" si="4"/>
         <v>259</v>
       </c>
-      <c r="J98" s="4">
+      <c r="J98">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3779,7 +3777,7 @@
         <f t="shared" si="4"/>
         <v>260</v>
       </c>
-      <c r="J99" s="4">
+      <c r="J99">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3811,7 +3809,7 @@
         <f t="shared" si="4"/>
         <v>261</v>
       </c>
-      <c r="J100" s="4">
+      <c r="J100">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3843,7 +3841,7 @@
         <f t="shared" si="4"/>
         <v>262</v>
       </c>
-      <c r="J101" s="4">
+      <c r="J101">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3875,7 +3873,7 @@
         <f t="shared" si="4"/>
         <v>263</v>
       </c>
-      <c r="J102" s="4">
+      <c r="J102">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3907,7 +3905,7 @@
         <f t="shared" si="4"/>
         <v>264</v>
       </c>
-      <c r="J103" s="4">
+      <c r="J103">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3939,7 +3937,7 @@
         <f t="shared" si="4"/>
         <v>264</v>
       </c>
-      <c r="J104" s="4">
+      <c r="J104">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3971,7 +3969,7 @@
         <f t="shared" si="4"/>
         <v>265</v>
       </c>
-      <c r="J105" s="4">
+      <c r="J105">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -4003,7 +4001,7 @@
         <f t="shared" si="4"/>
         <v>266</v>
       </c>
-      <c r="J106" s="4">
+      <c r="J106">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4035,7 +4033,7 @@
         <f t="shared" si="4"/>
         <v>266</v>
       </c>
-      <c r="J107" s="4">
+      <c r="J107">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -4067,7 +4065,7 @@
         <f t="shared" si="4"/>
         <v>267</v>
       </c>
-      <c r="J108" s="4">
+      <c r="J108">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4099,7 +4097,7 @@
         <f t="shared" si="4"/>
         <v>268</v>
       </c>
-      <c r="J109" s="4">
+      <c r="J109">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4131,7 +4129,7 @@
         <f t="shared" si="4"/>
         <v>268</v>
       </c>
-      <c r="J110" s="4">
+      <c r="J110">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4163,7 +4161,7 @@
         <f t="shared" si="4"/>
         <v>269</v>
       </c>
-      <c r="J111" s="4">
+      <c r="J111">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4195,7 +4193,7 @@
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
-      <c r="J112" s="4">
+      <c r="J112">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -4227,7 +4225,7 @@
         <f t="shared" si="4"/>
         <v>271</v>
       </c>
-      <c r="J113" s="4">
+      <c r="J113">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -4259,7 +4257,7 @@
         <f t="shared" si="4"/>
         <v>272</v>
       </c>
-      <c r="J114" s="4">
+      <c r="J114">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4291,7 +4289,7 @@
         <f t="shared" si="4"/>
         <v>273</v>
       </c>
-      <c r="J115" s="4">
+      <c r="J115">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4323,7 +4321,7 @@
         <f t="shared" si="4"/>
         <v>273</v>
       </c>
-      <c r="J116" s="4">
+      <c r="J116">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4355,7 +4353,7 @@
         <f t="shared" si="4"/>
         <v>274</v>
       </c>
-      <c r="J117" s="4">
+      <c r="J117">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4387,7 +4385,7 @@
         <f t="shared" si="4"/>
         <v>274</v>
       </c>
-      <c r="J118" s="4">
+      <c r="J118">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4419,7 +4417,7 @@
         <f t="shared" si="4"/>
         <v>275</v>
       </c>
-      <c r="J119" s="4">
+      <c r="J119">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4451,7 +4449,7 @@
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
-      <c r="J120" s="4">
+      <c r="J120">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -4483,7 +4481,7 @@
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
-      <c r="J121" s="4">
+      <c r="J121">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4515,7 +4513,7 @@
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
-      <c r="J122" s="4">
+      <c r="J122">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4547,7 +4545,7 @@
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
-      <c r="J123" s="4">
+      <c r="J123">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -4579,7 +4577,7 @@
         <f t="shared" si="4"/>
         <v>277</v>
       </c>
-      <c r="J124" s="4">
+      <c r="J124">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4611,7 +4609,7 @@
         <f t="shared" si="4"/>
         <v>278</v>
       </c>
-      <c r="J125" s="4">
+      <c r="J125">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4643,7 +4641,7 @@
         <f t="shared" si="4"/>
         <v>279</v>
       </c>
-      <c r="J126" s="4">
+      <c r="J126">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -4675,7 +4673,7 @@
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="J127" s="4">
+      <c r="J127">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -4707,7 +4705,7 @@
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="J128" s="4">
+      <c r="J128">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -4739,7 +4737,7 @@
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="J129" s="4">
+      <c r="J129">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4771,7 +4769,7 @@
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="J130" s="4">
+      <c r="J130">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4803,7 +4801,7 @@
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="J131" s="4">
+      <c r="J131">
         <f t="shared" ref="J131:J167" si="6">ROUND(A131*H$2,0) -I131</f>
         <v>7</v>
       </c>
@@ -4835,7 +4833,7 @@
         <f t="shared" ref="I132:I167" si="7">IF(E132="DEM",I131+1, I131)</f>
         <v>281</v>
       </c>
-      <c r="J132" s="4">
+      <c r="J132">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -4867,7 +4865,7 @@
         <f t="shared" si="7"/>
         <v>281</v>
       </c>
-      <c r="J133" s="4">
+      <c r="J133">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
@@ -4899,7 +4897,7 @@
         <f t="shared" si="7"/>
         <v>282</v>
       </c>
-      <c r="J134" s="4">
+      <c r="J134">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -4931,7 +4929,7 @@
         <f t="shared" si="7"/>
         <v>283</v>
       </c>
-      <c r="J135" s="4">
+      <c r="J135">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -4963,7 +4961,7 @@
         <f t="shared" si="7"/>
         <v>283</v>
       </c>
-      <c r="J136" s="4">
+      <c r="J136">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -4995,7 +4993,7 @@
         <f t="shared" si="7"/>
         <v>284</v>
       </c>
-      <c r="J137" s="4">
+      <c r="J137">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -5027,7 +5025,7 @@
         <f t="shared" si="7"/>
         <v>284</v>
       </c>
-      <c r="J138" s="4">
+      <c r="J138">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -5059,7 +5057,7 @@
         <f t="shared" si="7"/>
         <v>285</v>
       </c>
-      <c r="J139" s="4">
+      <c r="J139">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -5091,7 +5089,7 @@
         <f t="shared" si="7"/>
         <v>286</v>
       </c>
-      <c r="J140" s="4">
+      <c r="J140">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5123,7 +5121,7 @@
         <f t="shared" si="7"/>
         <v>287</v>
       </c>
-      <c r="J141" s="4">
+      <c r="J141">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5155,7 +5153,7 @@
         <f t="shared" si="7"/>
         <v>287</v>
       </c>
-      <c r="J142" s="4">
+      <c r="J142">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5187,7 +5185,7 @@
         <f t="shared" si="7"/>
         <v>288</v>
       </c>
-      <c r="J143" s="4">
+      <c r="J143">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5219,7 +5217,7 @@
         <f t="shared" si="7"/>
         <v>288</v>
       </c>
-      <c r="J144" s="4">
+      <c r="J144">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5251,7 +5249,7 @@
         <f t="shared" si="7"/>
         <v>289</v>
       </c>
-      <c r="J145" s="4">
+      <c r="J145">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5283,7 +5281,7 @@
         <f t="shared" si="7"/>
         <v>289</v>
       </c>
-      <c r="J146" s="4">
+      <c r="J146">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5315,7 +5313,7 @@
         <f t="shared" si="7"/>
         <v>290</v>
       </c>
-      <c r="J147" s="4">
+      <c r="J147">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5347,7 +5345,7 @@
         <f t="shared" si="7"/>
         <v>291</v>
       </c>
-      <c r="J148" s="4">
+      <c r="J148">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5379,7 +5377,7 @@
         <f t="shared" si="7"/>
         <v>291</v>
       </c>
-      <c r="J149" s="4">
+      <c r="J149">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -5411,7 +5409,7 @@
         <f t="shared" si="7"/>
         <v>292</v>
       </c>
-      <c r="J150" s="4">
+      <c r="J150">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5443,7 +5441,7 @@
         <f t="shared" si="7"/>
         <v>293</v>
       </c>
-      <c r="J151" s="4">
+      <c r="J151">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5475,7 +5473,7 @@
         <f t="shared" si="7"/>
         <v>293</v>
       </c>
-      <c r="J152" s="4">
+      <c r="J152">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5507,7 +5505,7 @@
         <f t="shared" si="7"/>
         <v>294</v>
       </c>
-      <c r="J153" s="4">
+      <c r="J153">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5539,7 +5537,7 @@
         <f t="shared" si="7"/>
         <v>295</v>
       </c>
-      <c r="J154" s="4">
+      <c r="J154">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -5571,7 +5569,7 @@
         <f t="shared" si="7"/>
         <v>296</v>
       </c>
-      <c r="J155" s="4">
+      <c r="J155">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -5603,7 +5601,7 @@
         <f t="shared" si="7"/>
         <v>296</v>
       </c>
-      <c r="J156" s="4">
+      <c r="J156">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5635,7 +5633,7 @@
         <f t="shared" si="7"/>
         <v>297</v>
       </c>
-      <c r="J157" s="4">
+      <c r="J157">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -5667,7 +5665,7 @@
         <f t="shared" si="7"/>
         <v>297</v>
       </c>
-      <c r="J158" s="4">
+      <c r="J158">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -5699,7 +5697,7 @@
         <f t="shared" si="7"/>
         <v>298</v>
       </c>
-      <c r="J159" s="4">
+      <c r="J159">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -5731,7 +5729,7 @@
         <f t="shared" si="7"/>
         <v>299</v>
       </c>
-      <c r="J160" s="4">
+      <c r="J160">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -5763,7 +5761,7 @@
         <f t="shared" si="7"/>
         <v>300</v>
       </c>
-      <c r="J161" s="4">
+      <c r="J161">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
@@ -5795,7 +5793,7 @@
         <f t="shared" si="7"/>
         <v>301</v>
       </c>
-      <c r="J162" s="4">
+      <c r="J162">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
@@ -5827,7 +5825,7 @@
         <f t="shared" si="7"/>
         <v>302</v>
       </c>
-      <c r="J163" s="4">
+      <c r="J163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -5859,7 +5857,7 @@
         <f t="shared" si="7"/>
         <v>303</v>
       </c>
-      <c r="J164" s="4">
+      <c r="J164">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -5891,7 +5889,7 @@
         <f t="shared" si="7"/>
         <v>303</v>
       </c>
-      <c r="J165" s="4">
+      <c r="J165">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -5923,7 +5921,7 @@
         <f t="shared" si="7"/>
         <v>304</v>
       </c>
-      <c r="J166" s="4">
+      <c r="J166">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -5955,7 +5953,7 @@
         <f t="shared" si="7"/>
         <v>305</v>
       </c>
-      <c r="J167" s="4">
+      <c r="J167">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>

</xml_diff>